<commit_message>
Added texts Forget to commit
</commit_message>
<xml_diff>
--- a/Dev/release/resources/Languages.xlsx
+++ b/Dev/release/resources/Languages.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="332">
   <si>
     <t>AboutEffekseer</t>
   </si>
@@ -999,6 +999,90 @@
   </si>
   <si>
     <t>Global Settings</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ShrinkAnchor</t>
+  </si>
+  <si>
+    <t>EnlargeAnchor_Desc</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ShrinkAnchor_Desc</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>アンカーの展開</t>
+    <rPh sb="5" eb="7">
+      <t>テンカイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>アンカーの縮退</t>
+    <rPh sb="5" eb="7">
+      <t>シュクタイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>値が急に変化するように
+アンカーをキーの位置に移動させる</t>
+    <rPh sb="0" eb="1">
+      <t>アタイ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>キュウ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>ヘンカ</t>
+    </rPh>
+    <rPh sb="20" eb="22">
+      <t>イチ</t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t>イドウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>値が滑らかに変化するように
+アンカーを広げる</t>
+    <rPh sb="0" eb="1">
+      <t>アタイ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>ナメ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>ヘンカ</t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t>ヒロ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>EnlargeAnchor</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Shrink anchor</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>To make the value change smoothly,
+extend the anchor</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Enlarge anchor</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>To make the value change suddenly
+move the anchor to the position of the key</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1042,10 +1126,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1351,10 +1438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C125"/>
+  <dimension ref="A1:C130"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="B121" sqref="B121"/>
+      <selection activeCell="B126" sqref="B126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2691,45 +2778,94 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A122" s="1" t="s">
-        <v>303</v>
+        <v>327</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>55</v>
+        <v>330</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.15">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" ht="27" x14ac:dyDescent="0.15">
       <c r="A123" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="B123" s="1" t="s">
-        <v>105</v>
+        <v>321</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>329</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>249</v>
+        <v>326</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A124" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" ht="27" x14ac:dyDescent="0.15">
+      <c r="A125" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A126" s="1"/>
+      <c r="B126" s="1"/>
+      <c r="C126" s="1"/>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A127" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A128" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A129" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="B124" s="1" t="s">
+      <c r="B129" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="C124" s="1" t="s">
+      <c r="C129" s="1" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A125" s="1" t="s">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A130" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="B125" s="1" t="s">
+      <c r="B130" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="C125" s="1" t="s">
+      <c r="C130" s="1" t="s">
         <v>264</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added functions to load and save a viewpoint
</commit_message>
<xml_diff>
--- a/Dev/release/resources/Languages.xlsx
+++ b/Dev/release/resources/Languages.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="810" uniqueCount="355">
   <si>
     <t>AboutEffekseer</t>
   </si>
@@ -596,9 +596,6 @@
   </si>
   <si>
     <t>振る舞い</t>
-  </si>
-  <si>
-    <t>カメラの種類"</t>
   </si>
   <si>
     <t>視点操作</t>
@@ -1172,6 +1169,40 @@
   </si>
   <si>
     <t>クリッピング</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Save</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Save</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Load</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Load</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>保存</t>
+    <rPh sb="0" eb="2">
+      <t>ホゾン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>読込</t>
+    <rPh sb="0" eb="2">
+      <t>ヨミコミ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>カメラの種類</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1527,10 +1558,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C137"/>
+  <dimension ref="A1:C140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
-      <selection activeCell="C138" sqref="C138"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1542,13 +1573,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B1" t="s">
+        <v>298</v>
+      </c>
+      <c r="C1" t="s">
         <v>299</v>
-      </c>
-      <c r="C1" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
@@ -1625,7 +1656,7 @@
         <v>12</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>194</v>
+        <v>354</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
@@ -1636,7 +1667,7 @@
         <v>14</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.15">
@@ -1647,7 +1678,7 @@
         <v>16</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.15">
@@ -1658,7 +1689,7 @@
         <v>18</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.15">
@@ -1669,7 +1700,7 @@
         <v>19</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.15">
@@ -1680,7 +1711,7 @@
         <v>20</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.15">
@@ -1691,7 +1722,7 @@
         <v>22</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.15">
@@ -1699,10 +1730,10 @@
         <v>23</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.15">
@@ -1713,7 +1744,7 @@
         <v>24</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.15">
@@ -1724,7 +1755,7 @@
         <v>25</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.15">
@@ -1735,7 +1766,7 @@
         <v>26</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.15">
@@ -1746,7 +1777,7 @@
         <v>28</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.15">
@@ -1757,7 +1788,7 @@
         <v>29</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.15">
@@ -1768,7 +1799,7 @@
         <v>31</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.15">
@@ -1779,7 +1810,7 @@
         <v>33</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.15">
@@ -1790,7 +1821,7 @@
         <v>35</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.15">
@@ -1801,7 +1832,7 @@
         <v>37</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.15">
@@ -1812,7 +1843,7 @@
         <v>39</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.15">
@@ -1823,7 +1854,7 @@
         <v>41</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.15">
@@ -1834,7 +1865,7 @@
         <v>42</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.15">
@@ -1845,7 +1876,7 @@
         <v>44</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.15">
@@ -1856,7 +1887,7 @@
         <v>45</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.15">
@@ -1867,7 +1898,7 @@
         <v>46</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="27" x14ac:dyDescent="0.15">
@@ -1878,7 +1909,7 @@
         <v>48</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.15">
@@ -1889,7 +1920,7 @@
         <v>49</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.15">
@@ -1900,7 +1931,7 @@
         <v>51</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.15">
@@ -1911,7 +1942,7 @@
         <v>52</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.15">
@@ -1922,7 +1953,7 @@
         <v>53</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.15">
@@ -1930,10 +1961,10 @@
         <v>54</v>
       </c>
       <c r="B36" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>341</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.15">
@@ -1944,7 +1975,7 @@
         <v>56</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.15">
@@ -1955,7 +1986,7 @@
         <v>57</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.15">
@@ -1977,7 +2008,7 @@
         <v>60</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.15">
@@ -1988,7 +2019,7 @@
         <v>62</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.15">
@@ -1999,7 +2030,7 @@
         <v>64</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.15">
@@ -2010,7 +2041,7 @@
         <v>66</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.15">
@@ -2021,7 +2052,7 @@
         <v>68</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.15">
@@ -2032,7 +2063,7 @@
         <v>70</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.15">
@@ -2043,7 +2074,7 @@
         <v>72</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.15">
@@ -2054,7 +2085,7 @@
         <v>74</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.15">
@@ -2065,7 +2096,7 @@
         <v>76</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.15">
@@ -2076,7 +2107,7 @@
         <v>78</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.15">
@@ -2087,7 +2118,7 @@
         <v>80</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.15">
@@ -2098,7 +2129,7 @@
         <v>82</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.15">
@@ -2109,7 +2140,7 @@
         <v>84</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.15">
@@ -2120,7 +2151,7 @@
         <v>86</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.15">
@@ -2131,7 +2162,7 @@
         <v>88</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.15">
@@ -2142,7 +2173,7 @@
         <v>90</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.15">
@@ -2153,7 +2184,7 @@
         <v>92</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.15">
@@ -2164,7 +2195,7 @@
         <v>94</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.15">
@@ -2175,7 +2206,7 @@
         <v>96</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.15">
@@ -2186,7 +2217,7 @@
         <v>97</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.15">
@@ -2197,7 +2228,7 @@
         <v>98</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.15">
@@ -2208,7 +2239,7 @@
         <v>100</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.15">
@@ -2219,7 +2250,7 @@
         <v>101</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.15">
@@ -2230,7 +2261,7 @@
         <v>102</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.15">
@@ -2241,7 +2272,7 @@
         <v>103</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.15">
@@ -2249,10 +2280,10 @@
         <v>104</v>
       </c>
       <c r="B65" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="C65" s="1" t="s">
         <v>308</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.15">
@@ -2263,7 +2294,7 @@
         <v>106</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.15">
@@ -2274,7 +2305,7 @@
         <v>108</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.15">
@@ -2285,7 +2316,7 @@
         <v>110</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.15">
@@ -2296,7 +2327,7 @@
         <v>112</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.15">
@@ -2307,7 +2338,7 @@
         <v>114</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.15">
@@ -2318,7 +2349,7 @@
         <v>116</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.15">
@@ -2329,7 +2360,7 @@
         <v>117</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.15">
@@ -2340,7 +2371,7 @@
         <v>119</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.15">
@@ -2351,7 +2382,7 @@
         <v>120</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.15">
@@ -2362,7 +2393,7 @@
         <v>121</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.15">
@@ -2373,7 +2404,7 @@
         <v>123</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.15">
@@ -2384,7 +2415,7 @@
         <v>124</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.15">
@@ -2395,7 +2426,7 @@
         <v>125</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.15">
@@ -2406,7 +2437,7 @@
         <v>127</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.15">
@@ -2414,10 +2445,10 @@
         <v>128</v>
       </c>
       <c r="B80" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="C80" s="1" t="s">
         <v>306</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.15">
@@ -2428,7 +2459,7 @@
         <v>130</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.15">
@@ -2439,7 +2470,7 @@
         <v>132</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.15">
@@ -2450,7 +2481,7 @@
         <v>133</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.15">
@@ -2461,7 +2492,7 @@
         <v>134</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.15">
@@ -2472,7 +2503,7 @@
         <v>135</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.15">
@@ -2483,7 +2514,7 @@
         <v>137</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.15">
@@ -2494,7 +2525,7 @@
         <v>139</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.15">
@@ -2505,7 +2536,7 @@
         <v>141</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.15">
@@ -2516,7 +2547,7 @@
         <v>142</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.15">
@@ -2527,7 +2558,7 @@
         <v>143</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.15">
@@ -2538,7 +2569,7 @@
         <v>144</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.15">
@@ -2549,7 +2580,7 @@
         <v>145</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.15">
@@ -2560,7 +2591,7 @@
         <v>146</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.15">
@@ -2571,7 +2602,7 @@
         <v>148</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.15">
@@ -2582,7 +2613,7 @@
         <v>150</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.15">
@@ -2593,7 +2624,7 @@
         <v>151</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.15">
@@ -2601,10 +2632,10 @@
         <v>152</v>
       </c>
       <c r="B97" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="C97" s="1" t="s">
         <v>338</v>
-      </c>
-      <c r="C97" s="1" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.15">
@@ -2615,7 +2646,7 @@
         <v>155</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.15">
@@ -2626,7 +2657,7 @@
         <v>156</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.15">
@@ -2637,7 +2668,7 @@
         <v>158</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.15">
@@ -2648,7 +2679,7 @@
         <v>160</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.15">
@@ -2659,7 +2690,7 @@
         <v>162</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.15">
@@ -2670,7 +2701,7 @@
         <v>164</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.15">
@@ -2681,7 +2712,7 @@
         <v>166</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.15">
@@ -2692,7 +2723,7 @@
         <v>168</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.15">
@@ -2703,7 +2734,7 @@
         <v>170</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.15">
@@ -2714,7 +2745,7 @@
         <v>171</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.15">
@@ -2725,7 +2756,7 @@
         <v>172</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.15">
@@ -2736,7 +2767,7 @@
         <v>174</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.15">
@@ -2747,7 +2778,7 @@
         <v>175</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.15">
@@ -2758,7 +2789,7 @@
         <v>176</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.15">
@@ -2769,7 +2800,7 @@
         <v>177</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.15">
@@ -2791,7 +2822,7 @@
         <v>181</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.15">
@@ -2802,7 +2833,7 @@
         <v>183</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.15">
@@ -2813,7 +2844,7 @@
         <v>184</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.15">
@@ -2824,7 +2855,7 @@
         <v>186</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.15">
@@ -2835,29 +2866,29 @@
         <v>187</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A119" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="B119" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="B119" s="1" t="s">
+      <c r="C119" s="1" t="s">
         <v>311</v>
-      </c>
-      <c r="C119" s="1" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A120" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="C120" s="1" t="s">
         <v>313</v>
-      </c>
-      <c r="B120" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="C120" s="1" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.15">
@@ -2867,46 +2898,46 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A122" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="123" spans="1:3" ht="27" x14ac:dyDescent="0.15">
       <c r="A123" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A124" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="27" x14ac:dyDescent="0.15">
       <c r="A125" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.15">
@@ -2916,35 +2947,35 @@
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A127" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="C127" t="s">
         <v>328</v>
-      </c>
-      <c r="B127" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="C127" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A128" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="C128" t="s">
         <v>331</v>
-      </c>
-      <c r="B128" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C128" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="129" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A129" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="B129" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="B129" s="1" t="s">
+      <c r="C129" s="1" t="s">
         <v>335</v>
-      </c>
-      <c r="C129" s="1" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.15">
@@ -2954,68 +2985,90 @@
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A131" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B131" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A132" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B132" s="1" t="s">
         <v>105</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A133" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B133" s="1" t="s">
         <v>153</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A134" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B134" s="1" t="s">
         <v>129</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A136" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="B136" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="B136" s="1" t="s">
+      <c r="C136" s="1" t="s">
         <v>344</v>
-      </c>
-      <c r="C136" s="1" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A137" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="B137" s="1" t="s">
         <v>346</v>
       </c>
-      <c r="B137" s="1" t="s">
+      <c r="C137" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="C137" s="1" t="s">
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A139" s="1" t="s">
         <v>348</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A140" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>353</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
make enabled to save recording settings into a project
</commit_message>
<xml_diff>
--- a/Dev/release/resources/Languages.xlsx
+++ b/Dev/release/resources/Languages.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="810" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="364">
   <si>
     <t>AboutEffekseer</t>
   </si>
@@ -1203,6 +1203,51 @@
   </si>
   <si>
     <t>カメラの種類</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Effekseer Project</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Setting save destination</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>設定保存先</t>
+    <rPh sb="0" eb="2">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>ホゾン</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>サキ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Effekseer Application</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Effekseerアプリケーション</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>プロジェクト</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>StorageGlobal</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>StorageLocal</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>StorageTarget</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1558,16 +1603,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C140"/>
+  <dimension ref="A1:C144"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
+      <selection activeCell="A142" sqref="A142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="34.5" customWidth="1"/>
-    <col min="2" max="2" width="80.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.42578125" customWidth="1"/>
+    <col min="2" max="2" width="80.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="69" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3071,6 +3116,39 @@
         <v>353</v>
       </c>
     </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A142" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A143" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A144" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="B144" t="s">
+        <v>355</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>360</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
implementing material and dynamic parameter rename an effect's texture
</commit_message>
<xml_diff>
--- a/Dev/release/resources/Languages.xlsx
+++ b/Dev/release/resources/Languages.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="367">
   <si>
     <t>AboutEffekseer</t>
   </si>
@@ -1248,6 +1248,21 @@
   </si>
   <si>
     <t>StorageTarget</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Dynamic parameter</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>動的パラメーター</t>
+    <rPh sb="0" eb="2">
+      <t>ドウテキ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>DynamicParameter_Name</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1603,16 +1618,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C144"/>
+  <dimension ref="A1:C146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
-      <selection activeCell="A142" sqref="A142"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="A123" sqref="A123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="34.42578125" customWidth="1"/>
-    <col min="2" max="2" width="80.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.375" customWidth="1"/>
+    <col min="2" max="2" width="80.25" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="69" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2943,209 +2958,225 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A122" s="1" t="s">
-        <v>322</v>
+        <v>366</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>325</v>
+        <v>364</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" ht="27" x14ac:dyDescent="0.15">
-      <c r="A123" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="B123" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="C123" s="1" t="s">
-        <v>321</v>
-      </c>
+        <v>365</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A123" s="1"/>
+      <c r="B123" s="1"/>
+      <c r="C123" s="1"/>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A124" s="1" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="27" x14ac:dyDescent="0.15">
       <c r="A125" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A126" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" ht="27" x14ac:dyDescent="0.15">
+      <c r="A127" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="B125" s="2" t="s">
+      <c r="B127" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="C125" s="1" t="s">
+      <c r="C127" s="1" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A126" s="1"/>
-      <c r="B126" s="2"/>
-      <c r="C126" s="1"/>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A127" s="1" t="s">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A128" s="1"/>
+      <c r="B128" s="2"/>
+      <c r="C128" s="1"/>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A129" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="B127" s="1" t="s">
+      <c r="B129" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="C127" t="s">
+      <c r="C129" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A128" s="1" t="s">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A130" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="B128" s="1" t="s">
+      <c r="B130" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="C128" t="s">
+      <c r="C130" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="129" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A129" s="1" t="s">
+    <row r="131" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A131" s="1" t="s">
         <v>333</v>
       </c>
-      <c r="B129" s="1" t="s">
+      <c r="B131" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="C129" s="1" t="s">
+      <c r="C131" s="1" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A130" s="1"/>
-      <c r="B130" s="1"/>
-      <c r="C130" s="1"/>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A131" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="B131" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C131" s="1" t="s">
-        <v>220</v>
-      </c>
-    </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A132" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="B132" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C132" s="1" t="s">
-        <v>247</v>
-      </c>
+      <c r="A132" s="1"/>
+      <c r="B132" s="1"/>
+      <c r="C132" s="1"/>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A133" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>153</v>
+        <v>55</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>277</v>
+        <v>220</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A134" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>129</v>
+        <v>105</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>262</v>
+        <v>247</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A135" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A136" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A138" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="B136" s="1" t="s">
+      <c r="B138" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="C136" s="1" t="s">
+      <c r="C138" s="1" t="s">
         <v>344</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A137" s="1" t="s">
-        <v>345</v>
-      </c>
-      <c r="B137" s="1" t="s">
-        <v>346</v>
-      </c>
-      <c r="C137" s="1" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A139" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A141" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="B139" s="1" t="s">
+      <c r="B141" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="C139" s="1" t="s">
+      <c r="C141" s="1" t="s">
         <v>352</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A140" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="B140" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="C140" s="1" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A142" s="1" t="s">
-        <v>363</v>
+        <v>350</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A143" s="1" t="s">
-        <v>361</v>
-      </c>
-      <c r="B143" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="C143" s="1" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A144" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A145" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="C145" s="1" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A146" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="B144" t="s">
+      <c r="B146" t="s">
         <v>355</v>
       </c>
-      <c r="C144" s="1" t="s">
+      <c r="C146" s="1" t="s">
         <v>360</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Improve recording UI. Documentation work.
</commit_message>
<xml_diff>
--- a/Dev/release/resources/Languages.xlsx
+++ b/Dev/release/resources/Languages.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="370">
   <si>
     <t>AboutEffekseer</t>
   </si>
@@ -1263,6 +1263,24 @@
   </si>
   <si>
     <t>DynamicParameter_Name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>GenerateAlpha2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Generate alpha(Blend+Add)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>生成(ブレンド+加算)</t>
+    <rPh sb="0" eb="2">
+      <t>セイセイ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>カサン</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1618,10 +1636,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C146"/>
+  <dimension ref="A1:C147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="A123" sqref="A123"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1996,560 +2014,560 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
-        <v>52</v>
+        <v>367</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>52</v>
+        <v>368</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>218</v>
+        <v>369</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>340</v>
+        <v>53</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>341</v>
+        <v>219</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>56</v>
+        <v>340</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>221</v>
+        <v>341</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>188</v>
+        <v>222</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A40" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>60</v>
+        <v>1</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>223</v>
+        <v>188</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A41" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A42" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A43" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>203</v>
+        <v>225</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A44" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>226</v>
+        <v>203</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A45" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A46" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A47" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A49" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A50" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A51" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A52" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A53" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A54" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A55" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A56" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A57" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A58" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A59" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A60" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A61" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A62" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A63" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A64" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A65" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>307</v>
+        <v>103</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>308</v>
+        <v>246</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A66" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>106</v>
+        <v>307</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>248</v>
+        <v>308</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A67" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A68" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A69" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A70" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A71" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A72" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A73" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A74" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A75" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A76" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A77" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A78" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A79" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A80" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>305</v>
+        <v>127</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>306</v>
+        <v>261</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A81" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>130</v>
+        <v>305</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>263</v>
+        <v>306</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A82" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A83" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A84" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>265</v>
@@ -2557,21 +2575,21 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A85" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A86" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>266</v>
@@ -2579,604 +2597,615 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A87" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A88" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A89" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A90" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A91" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A92" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A93" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A94" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A95" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A96" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A97" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>337</v>
+        <v>151</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>338</v>
+        <v>276</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A98" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>155</v>
+        <v>337</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>278</v>
+        <v>338</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A99" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A100" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A101" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A102" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A103" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A104" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A105" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A106" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A107" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A108" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A109" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A110" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A111" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A112" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A113" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>179</v>
+        <v>292</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A114" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>293</v>
+        <v>179</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A115" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A116" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A117" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A118" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A119" s="1" t="s">
-        <v>309</v>
+        <v>187</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>310</v>
+        <v>187</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>311</v>
+        <v>297</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A120" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A121" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="B120" s="1" t="s">
+      <c r="B121" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="C120" s="1" t="s">
+      <c r="C121" s="1" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A121" s="1"/>
-      <c r="B121" s="1"/>
-      <c r="C121" s="1"/>
-    </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A122" s="1" t="s">
+      <c r="A122" s="1"/>
+      <c r="B122" s="1"/>
+      <c r="C122" s="1"/>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A123" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="B122" s="1" t="s">
+      <c r="B123" s="1" t="s">
         <v>364</v>
       </c>
-      <c r="C122" s="1" t="s">
+      <c r="C123" s="1" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A123" s="1"/>
-      <c r="B123" s="1"/>
-      <c r="C123" s="1"/>
-    </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A124" s="1" t="s">
+      <c r="A124" s="1"/>
+      <c r="B124" s="1"/>
+      <c r="C124" s="1"/>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A125" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="B124" s="1" t="s">
+      <c r="B125" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="C124" s="1" t="s">
+      <c r="C125" s="1" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="125" spans="1:3" ht="27" x14ac:dyDescent="0.15">
-      <c r="A125" s="1" t="s">
+    <row r="126" spans="1:3" ht="27" x14ac:dyDescent="0.15">
+      <c r="A126" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="B125" s="2" t="s">
+      <c r="B126" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="C125" s="1" t="s">
+      <c r="C126" s="1" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A126" s="1" t="s">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A127" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="B126" s="1" t="s">
+      <c r="B127" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="C126" s="1" t="s">
+      <c r="C127" s="1" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="127" spans="1:3" ht="27" x14ac:dyDescent="0.15">
-      <c r="A127" s="1" t="s">
+    <row r="128" spans="1:3" ht="27" x14ac:dyDescent="0.15">
+      <c r="A128" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="B127" s="2" t="s">
+      <c r="B128" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="C127" s="1" t="s">
+      <c r="C128" s="1" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A128" s="1"/>
-      <c r="B128" s="2"/>
-      <c r="C128" s="1"/>
-    </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A129" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="B129" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="C129" t="s">
-        <v>328</v>
-      </c>
+      <c r="A129" s="1"/>
+      <c r="B129" s="2"/>
+      <c r="C129" s="1"/>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A130" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="C130" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A131" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="B130" s="1" t="s">
+      <c r="B131" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="C130" t="s">
+      <c r="C131" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="131" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A131" s="1" t="s">
+    <row r="132" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A132" s="1" t="s">
         <v>333</v>
       </c>
-      <c r="B131" s="1" t="s">
+      <c r="B132" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="C131" s="1" t="s">
+      <c r="C132" s="1" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A132" s="1"/>
-      <c r="B132" s="1"/>
-      <c r="C132" s="1"/>
-    </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A133" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="B133" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C133" s="1" t="s">
-        <v>220</v>
-      </c>
+      <c r="A133" s="1"/>
+      <c r="B133" s="1"/>
+      <c r="C133" s="1"/>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A134" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>105</v>
+        <v>55</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>247</v>
+        <v>220</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A135" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>153</v>
+        <v>105</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>277</v>
+        <v>247</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A136" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A137" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="B136" s="1" t="s">
+      <c r="B137" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="C136" s="1" t="s">
+      <c r="C137" s="1" t="s">
         <v>262</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A138" s="1" t="s">
-        <v>342</v>
-      </c>
-      <c r="B138" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="C138" s="1" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A139" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A140" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="B139" s="1" t="s">
+      <c r="B140" s="1" t="s">
         <v>346</v>
       </c>
-      <c r="C139" s="1" t="s">
+      <c r="C140" s="1" t="s">
         <v>347</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A141" s="1" t="s">
-        <v>348</v>
-      </c>
-      <c r="B141" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="C141" s="1" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A142" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A143" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="B142" s="1" t="s">
+      <c r="B143" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="C142" s="1" t="s">
+      <c r="C143" s="1" t="s">
         <v>353</v>
-      </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A144" s="1" t="s">
-        <v>363</v>
-      </c>
-      <c r="B144" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="C144" s="1" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A145" s="1" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A146" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="C146" s="1" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A147" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="B146" t="s">
+      <c r="B147" t="s">
         <v>355</v>
       </c>
-      <c r="C146" s="1" t="s">
+      <c r="C147" s="1" t="s">
         <v>360</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added a compile error texts
</commit_message>
<xml_diff>
--- a/Dev/release/resources/Languages.xlsx
+++ b/Dev/release/resources/Languages.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="411">
   <si>
     <t>AboutEffekseer</t>
   </si>
@@ -1361,6 +1361,174 @@
   </si>
   <si>
     <t>efkmat</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> : Line {0} Col {1}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> : 行 {0} 列 {1}</t>
+    <rPh sb="3" eb="4">
+      <t>ギョウ</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>レツ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>CompileErrror_InvalidToken</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>CompileErrror_InvalidEoF</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Invalid token {0} is found</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Unexpected end is found</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>予期せぬ終了が見つかりました</t>
+    <rPh sb="0" eb="2">
+      <t>ヨキ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>シュウリョウ</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>ミ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>無効なトークン {0} が見つかりました</t>
+    <rPh sb="0" eb="2">
+      <t>ムコウ</t>
+    </rPh>
+    <rPh sb="13" eb="14">
+      <t>ミ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>CompileError_InvalidOperation</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Invalid operation is found</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>無効な操作が見つかりました</t>
+    <rPh sb="0" eb="2">
+      <t>ムコウ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>ソウサ</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>ミ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>CompileError_ArgSize</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>引数の個数が間違っています。要求 {0} 実際 {1}</t>
+    <rPh sb="0" eb="2">
+      <t>ヒキスウ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>コスウ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>マチガ</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>ヨウキュウ</t>
+    </rPh>
+    <rPh sb="21" eb="23">
+      <t>ジッサイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>The number of arguments is wrong. Expected {0} Actual {1}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Invalid substitution is found</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>無効な代入が見つかりました</t>
+    <rPh sb="0" eb="2">
+      <t>ムコウ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>ダイニュウ</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>ミ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>CompileError_InvalidSubstitution</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Unkwon function {0} is found</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>知らない関数 {0} が見つかりました</t>
+    <rPh sb="0" eb="1">
+      <t>シ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>カンスウ</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t>ミ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>CompileError_UnknownFunction</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>CompileError_UnknownValue</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Unkwon value {0} is found</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>知らない値 {0} が見つかりました</t>
+    <rPh sb="0" eb="1">
+      <t>シ</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>アタイ</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>ミ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>CompilePosition</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1716,10 +1884,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C156"/>
+  <dimension ref="A1:C165"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
-      <selection activeCell="C157" sqref="C157"/>
+      <selection activeCell="A159" sqref="A159:A165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3360,6 +3528,94 @@
         <v>386</v>
       </c>
     </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A158" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="B158" t="s">
+        <v>387</v>
+      </c>
+      <c r="C158" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A159" t="s">
+        <v>389</v>
+      </c>
+      <c r="B159" t="s">
+        <v>391</v>
+      </c>
+      <c r="C159" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A160" t="s">
+        <v>390</v>
+      </c>
+      <c r="B160" t="s">
+        <v>392</v>
+      </c>
+      <c r="C160" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A161" t="s">
+        <v>395</v>
+      </c>
+      <c r="B161" t="s">
+        <v>396</v>
+      </c>
+      <c r="C161" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A162" t="s">
+        <v>398</v>
+      </c>
+      <c r="B162" t="s">
+        <v>400</v>
+      </c>
+      <c r="C162" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A163" t="s">
+        <v>403</v>
+      </c>
+      <c r="B163" t="s">
+        <v>401</v>
+      </c>
+      <c r="C163" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A164" t="s">
+        <v>406</v>
+      </c>
+      <c r="B164" t="s">
+        <v>404</v>
+      </c>
+      <c r="C164" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A165" t="s">
+        <v>407</v>
+      </c>
+      <c r="B165" t="s">
+        <v>408</v>
+      </c>
+      <c r="C165" t="s">
+        <v>409</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add rename context to node tree
</commit_message>
<xml_diff>
--- a/Dev/release/resources/Languages.xlsx
+++ b/Dev/release/resources/Languages.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10917"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D943401B-DEC4-3846-979B-F81D7859C83C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="41480" windowHeight="20360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="417">
   <si>
     <t>AboutEffekseer</t>
   </si>
@@ -1531,22 +1532,40 @@
     <t>CompilePosition</t>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>RenameNode</t>
+  </si>
+  <si>
+    <t>Rename</t>
+  </si>
+  <si>
+    <t>名称の変更</t>
+  </si>
+  <si>
+    <t>InternalRenameNode</t>
+  </si>
+  <si>
+    <t>Cancel</t>
+  </si>
+  <si>
+    <t>キャンセル</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -1582,7 +1601,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="標準" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -1598,7 +1617,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1673,6 +1692,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1708,6 +1744,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1883,21 +1936,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C165"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
-      <selection activeCell="A159" sqref="A159:A165"/>
+    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
+      <selection activeCell="A168" sqref="A168:C168"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34.375" customWidth="1"/>
-    <col min="2" max="2" width="80.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.33203125" customWidth="1"/>
+    <col min="2" max="2" width="80.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="69" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>300</v>
       </c>
@@ -1908,7 +1961,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1919,7 +1972,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1930,7 +1983,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1941,7 +1994,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -1952,7 +2005,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -1963,7 +2016,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -1974,7 +2027,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -1985,7 +2038,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
@@ -1996,7 +2049,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
@@ -2007,7 +2060,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
@@ -2018,7 +2071,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
@@ -2029,7 +2082,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>20</v>
       </c>
@@ -2040,7 +2093,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>21</v>
       </c>
@@ -2051,7 +2104,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>23</v>
       </c>
@@ -2062,7 +2115,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>24</v>
       </c>
@@ -2073,7 +2126,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>25</v>
       </c>
@@ -2084,7 +2137,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>26</v>
       </c>
@@ -2095,7 +2148,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>27</v>
       </c>
@@ -2106,7 +2159,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>29</v>
       </c>
@@ -2117,7 +2170,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>30</v>
       </c>
@@ -2128,7 +2181,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>32</v>
       </c>
@@ -2139,7 +2192,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>34</v>
       </c>
@@ -2150,7 +2203,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>36</v>
       </c>
@@ -2161,7 +2214,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>38</v>
       </c>
@@ -2172,7 +2225,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>40</v>
       </c>
@@ -2183,7 +2236,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>42</v>
       </c>
@@ -2194,7 +2247,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>43</v>
       </c>
@@ -2205,7 +2258,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>45</v>
       </c>
@@ -2216,7 +2269,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>46</v>
       </c>
@@ -2227,7 +2280,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="27" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>47</v>
       </c>
@@ -2238,7 +2291,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>49</v>
       </c>
@@ -2249,7 +2302,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>50</v>
       </c>
@@ -2260,7 +2313,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>367</v>
       </c>
@@ -2271,7 +2324,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>52</v>
       </c>
@@ -2282,7 +2335,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>53</v>
       </c>
@@ -2293,7 +2346,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>54</v>
       </c>
@@ -2304,7 +2357,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>56</v>
       </c>
@@ -2315,7 +2368,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>57</v>
       </c>
@@ -2326,7 +2379,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>58</v>
       </c>
@@ -2337,7 +2390,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>59</v>
       </c>
@@ -2348,7 +2401,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>61</v>
       </c>
@@ -2359,7 +2412,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>63</v>
       </c>
@@ -2370,7 +2423,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>65</v>
       </c>
@@ -2381,7 +2434,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>67</v>
       </c>
@@ -2392,7 +2445,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>69</v>
       </c>
@@ -2403,7 +2456,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>71</v>
       </c>
@@ -2414,7 +2467,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>73</v>
       </c>
@@ -2425,7 +2478,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>75</v>
       </c>
@@ -2436,7 +2489,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>77</v>
       </c>
@@ -2447,7 +2500,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>79</v>
       </c>
@@ -2458,7 +2511,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>81</v>
       </c>
@@ -2469,7 +2522,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>83</v>
       </c>
@@ -2480,7 +2533,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>85</v>
       </c>
@@ -2491,7 +2544,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>87</v>
       </c>
@@ -2502,7 +2555,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>89</v>
       </c>
@@ -2513,7 +2566,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>91</v>
       </c>
@@ -2524,7 +2577,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>93</v>
       </c>
@@ -2535,7 +2588,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>95</v>
       </c>
@@ -2546,1074 +2599,1107 @@
         <v>240</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A61" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A62" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B62" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="C62" s="1" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A61" s="1" t="s">
+    <row r="63" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B63" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C61" s="1" t="s">
+      <c r="C63" s="1" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A62" s="1" t="s">
+    <row r="64" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A64" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="B64" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C62" s="1" t="s">
+      <c r="C64" s="1" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A63" s="1" t="s">
+    <row r="65" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A65" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="B65" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="C63" s="1" t="s">
+      <c r="C65" s="1" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A64" s="1" t="s">
+    <row r="66" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A66" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="B66" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C64" s="1" t="s">
+      <c r="C66" s="1" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A65" s="1" t="s">
+    <row r="67" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A67" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="B67" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C65" s="1" t="s">
+      <c r="C67" s="1" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A66" s="1" t="s">
+    <row r="68" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A68" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="B68" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="C66" s="1" t="s">
+      <c r="C68" s="1" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A67" s="1" t="s">
+    <row r="69" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A69" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="B69" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C67" s="1" t="s">
+      <c r="C69" s="1" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A68" s="1" t="s">
+    <row r="70" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A70" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B68" s="1" t="s">
+      <c r="B70" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C68" s="1" t="s">
+      <c r="C70" s="1" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A69" s="1" t="s">
+    <row r="71" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A71" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="B71" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C69" s="1" t="s">
+      <c r="C71" s="1" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A70" s="1" t="s">
+    <row r="72" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A72" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="B72" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C70" s="1" t="s">
+      <c r="C72" s="1" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A71" s="1" t="s">
+    <row r="73" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A73" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="B73" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="C71" s="1" t="s">
+      <c r="C73" s="1" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A72" s="1" t="s">
+    <row r="74" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A74" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B72" s="1" t="s">
+      <c r="B74" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="C72" s="1" t="s">
+      <c r="C74" s="1" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A73" s="1" t="s">
+    <row r="75" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A75" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B73" s="1" t="s">
+      <c r="B75" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="C73" s="1" t="s">
+      <c r="C75" s="1" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A74" s="1" t="s">
+    <row r="76" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A76" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B74" s="1" t="s">
+      <c r="B76" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="C74" s="1" t="s">
+      <c r="C76" s="1" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A75" s="1" t="s">
+    <row r="77" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A77" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B75" s="1" t="s">
+      <c r="B77" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="C75" s="1" t="s">
+      <c r="C77" s="1" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A76" s="1" t="s">
+    <row r="78" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A78" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="B78" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="C76" s="1" t="s">
+      <c r="C78" s="1" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A77" s="1" t="s">
+    <row r="79" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A79" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B77" s="1" t="s">
+      <c r="B79" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="C77" s="1" t="s">
+      <c r="C79" s="1" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A78" s="1" t="s">
+    <row r="80" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A80" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B78" s="1" t="s">
+      <c r="B80" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="C78" s="1" t="s">
+      <c r="C80" s="1" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A79" s="1" t="s">
+    <row r="81" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A81" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B79" s="1" t="s">
+      <c r="B81" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="C79" s="1" t="s">
+      <c r="C81" s="1" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A80" s="1" t="s">
+    <row r="82" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A82" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B80" s="1" t="s">
+      <c r="B82" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C80" s="1" t="s">
+      <c r="C82" s="1" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A81" s="1" t="s">
+    <row r="83" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A83" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B81" s="1" t="s">
+      <c r="B83" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="C81" s="1" t="s">
+      <c r="C83" s="1" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A82" s="1" t="s">
+    <row r="84" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A84" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B82" s="1" t="s">
+      <c r="B84" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="C82" s="1" t="s">
+      <c r="C84" s="1" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A83" s="1" t="s">
+    <row r="85" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A85" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B83" s="1" t="s">
+      <c r="B85" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C83" s="1" t="s">
+      <c r="C85" s="1" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A84" s="1" t="s">
+    <row r="86" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A86" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B84" s="1" t="s">
+      <c r="B86" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="C84" s="1" t="s">
+      <c r="C86" s="1" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A85" s="1" t="s">
+    <row r="87" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A87" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B85" s="1" t="s">
+      <c r="B87" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="C85" s="1" t="s">
+      <c r="C87" s="1" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A86" s="1" t="s">
+    <row r="88" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A88" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B86" s="1" t="s">
+      <c r="B88" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C86" s="1" t="s">
+      <c r="C88" s="1" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A87" s="1" t="s">
+    <row r="89" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A89" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B87" s="1" t="s">
+      <c r="B89" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C87" s="1" t="s">
+      <c r="C89" s="1" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A88" s="1" t="s">
+    <row r="90" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A90" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B88" s="1" t="s">
+      <c r="B90" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="C88" s="1" t="s">
+      <c r="C90" s="1" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A89" s="1" t="s">
+    <row r="91" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A91" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B89" s="1" t="s">
+      <c r="B91" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="C89" s="1" t="s">
+      <c r="C91" s="1" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A90" s="1" t="s">
+    <row r="92" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A92" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B90" s="1" t="s">
+      <c r="B92" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="C90" s="1" t="s">
+      <c r="C92" s="1" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A91" s="1" t="s">
+    <row r="93" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A93" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B91" s="1" t="s">
+      <c r="B93" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="C91" s="1" t="s">
+      <c r="C93" s="1" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A92" s="1" t="s">
+    <row r="94" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A94" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B92" s="1" t="s">
+      <c r="B94" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="C92" s="1" t="s">
+      <c r="C94" s="1" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A93" s="1" t="s">
+    <row r="95" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A95" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B93" s="1" t="s">
+      <c r="B95" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="C93" s="1" t="s">
+      <c r="C95" s="1" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A94" s="1" t="s">
+    <row r="96" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A96" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B94" s="1" t="s">
+      <c r="B96" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="C94" s="1" t="s">
+      <c r="C96" s="1" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A95" s="1" t="s">
+    <row r="97" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A97" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B95" s="1" t="s">
+      <c r="B97" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C95" s="1" t="s">
+      <c r="C97" s="1" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A96" s="1" t="s">
+    <row r="98" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A98" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="B96" s="1" t="s">
+      <c r="B98" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="C96" s="1" t="s">
+      <c r="C98" s="1" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A97" s="1" t="s">
+    <row r="99" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A99" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B97" s="1" t="s">
+      <c r="B99" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="C97" s="1" t="s">
+      <c r="C99" s="1" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A98" s="1" t="s">
+    <row r="100" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A100" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="B98" s="1" t="s">
+      <c r="B100" s="1" t="s">
         <v>337</v>
       </c>
-      <c r="C98" s="1" t="s">
+      <c r="C100" s="1" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A99" s="1" t="s">
+    <row r="101" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A101" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="B99" s="1" t="s">
+      <c r="B101" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="C99" s="1" t="s">
+      <c r="C101" s="1" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A100" s="1" t="s">
+    <row r="102" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A102" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="B100" s="1" t="s">
+      <c r="B102" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="C100" s="1" t="s">
+      <c r="C102" s="1" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A101" s="1" t="s">
+    <row r="103" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A103" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="B101" s="1" t="s">
+      <c r="B103" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="C101" s="1" t="s">
+      <c r="C103" s="1" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A102" s="1" t="s">
+    <row r="104" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A104" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="B102" s="1" t="s">
+      <c r="B104" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="C102" s="1" t="s">
+      <c r="C104" s="1" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A103" s="1" t="s">
+    <row r="105" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A105" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="B103" s="1" t="s">
+      <c r="B105" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C103" s="1" t="s">
+      <c r="C105" s="1" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A104" s="1" t="s">
+    <row r="106" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A106" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B104" s="1" t="s">
+      <c r="B106" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="C104" s="1" t="s">
+      <c r="C106" s="1" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A105" s="1" t="s">
+    <row r="107" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A107" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="B105" s="1" t="s">
+      <c r="B107" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="C105" s="1" t="s">
+      <c r="C107" s="1" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A106" s="1" t="s">
+    <row r="108" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A108" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="B106" s="1" t="s">
+      <c r="B108" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="C106" s="1" t="s">
+      <c r="C108" s="1" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A107" s="1" t="s">
+    <row r="109" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A109" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="B107" s="1" t="s">
+      <c r="B109" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="C107" s="1" t="s">
+      <c r="C109" s="1" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A108" s="1" t="s">
+    <row r="110" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A110" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="B108" s="1" t="s">
+      <c r="B110" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="C108" s="1" t="s">
+      <c r="C110" s="1" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A109" s="1" t="s">
+    <row r="111" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A111" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="B109" s="1" t="s">
+      <c r="B111" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="C109" s="1" t="s">
+      <c r="C111" s="1" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A110" s="1" t="s">
+    <row r="112" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A112" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="B110" s="1" t="s">
+      <c r="B112" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="C110" s="1" t="s">
+      <c r="C112" s="1" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A111" s="1" t="s">
+    <row r="113" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A113" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="B111" s="1" t="s">
+      <c r="B113" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="C111" s="1" t="s">
+      <c r="C113" s="1" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A112" s="1" t="s">
+    <row r="114" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A114" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="B112" s="1" t="s">
+      <c r="B114" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="C112" s="1" t="s">
+      <c r="C114" s="1" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A113" s="1" t="s">
+    <row r="115" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A115" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="B113" s="1" t="s">
+      <c r="B115" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="C113" s="1" t="s">
+      <c r="C115" s="1" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A114" s="1" t="s">
+    <row r="116" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A116" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="B114" s="1" t="s">
+      <c r="B116" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="C114" s="1" t="s">
+      <c r="C116" s="1" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A115" s="1" t="s">
+    <row r="117" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A117" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="B115" s="1" t="s">
+      <c r="B117" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="C115" s="1" t="s">
+      <c r="C117" s="1" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A116" s="1" t="s">
+    <row r="118" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A118" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="B116" s="1" t="s">
+      <c r="B118" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="C116" s="1" t="s">
+      <c r="C118" s="1" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A117" s="1" t="s">
+    <row r="119" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A119" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="B117" s="1" t="s">
+      <c r="B119" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="C117" s="1" t="s">
+      <c r="C119" s="1" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A118" s="1" t="s">
+    <row r="120" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A120" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="B118" s="1" t="s">
+      <c r="B120" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="C118" s="1" t="s">
+      <c r="C120" s="1" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A119" s="1" t="s">
+    <row r="121" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A121" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="B119" s="1" t="s">
+      <c r="B121" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="C119" s="1" t="s">
+      <c r="C121" s="1" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A120" s="1" t="s">
+    <row r="122" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A122" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="B120" s="1" t="s">
+      <c r="B122" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="C120" s="1" t="s">
+      <c r="C122" s="1" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A121" s="1" t="s">
+    <row r="123" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A123" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="B121" s="1" t="s">
+      <c r="B123" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="C121" s="1" t="s">
+      <c r="C123" s="1" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A122" s="1"/>
-      <c r="B122" s="1"/>
-      <c r="C122" s="1"/>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A123" s="1" t="s">
-        <v>366</v>
-      </c>
-      <c r="B123" s="1" t="s">
-        <v>364</v>
-      </c>
-      <c r="C123" s="1" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124" s="1"/>
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="125" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A126" s="1"/>
+      <c r="B126" s="1"/>
+      <c r="C126" s="1"/>
+    </row>
+    <row r="127" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A127" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="B125" s="1" t="s">
+      <c r="B127" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="C125" s="1" t="s">
+      <c r="C127" s="1" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="126" spans="1:3" ht="27" x14ac:dyDescent="0.15">
-      <c r="A126" s="1" t="s">
+    <row r="128" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A128" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="B126" s="2" t="s">
+      <c r="B128" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="C126" s="1" t="s">
+      <c r="C128" s="1" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A127" s="1" t="s">
+    <row r="129" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A129" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="B127" s="1" t="s">
+      <c r="B129" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="C127" s="1" t="s">
+      <c r="C129" s="1" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="128" spans="1:3" ht="27" x14ac:dyDescent="0.15">
-      <c r="A128" s="1" t="s">
+    <row r="130" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A130" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="B128" s="2" t="s">
+      <c r="B130" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="C128" s="1" t="s">
+      <c r="C130" s="1" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A129" s="1"/>
-      <c r="B129" s="2"/>
-      <c r="C129" s="1"/>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A130" s="1" t="s">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A131" s="1"/>
+      <c r="B131" s="2"/>
+      <c r="C131" s="1"/>
+    </row>
+    <row r="132" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A132" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="B130" s="1" t="s">
+      <c r="B132" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="C130" t="s">
+      <c r="C132" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A131" s="1" t="s">
+    <row r="133" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A133" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="B131" s="1" t="s">
+      <c r="B133" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="C131" t="s">
+      <c r="C133" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="132" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A132" s="1" t="s">
+    <row r="134" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A134" s="1" t="s">
         <v>333</v>
       </c>
-      <c r="B132" s="1" t="s">
+      <c r="B134" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="C132" s="1" t="s">
+      <c r="C134" s="1" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A133" s="1"/>
-      <c r="B133" s="1"/>
-      <c r="C133" s="1"/>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A134" s="1" t="s">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A135" s="1"/>
+      <c r="B135" s="1"/>
+      <c r="C135" s="1"/>
+    </row>
+    <row r="136" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A136" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="B134" s="1" t="s">
+      <c r="B136" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C134" s="1" t="s">
+      <c r="C136" s="1" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A135" s="1" t="s">
+    <row r="137" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A137" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="B135" s="1" t="s">
+      <c r="B137" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C135" s="1" t="s">
+      <c r="C137" s="1" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A136" s="1" t="s">
+    <row r="138" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A138" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="B136" s="1" t="s">
+      <c r="B138" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="C136" s="1" t="s">
+      <c r="C138" s="1" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A137" s="1" t="s">
+    <row r="139" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A139" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="B137" s="1" t="s">
+      <c r="B139" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="C137" s="1" t="s">
+      <c r="C139" s="1" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A138" s="1"/>
-      <c r="B138" s="1"/>
-      <c r="C138" s="1"/>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A140" s="1" t="s">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A140" s="1"/>
+      <c r="B140" s="1"/>
+      <c r="C140" s="1"/>
+    </row>
+    <row r="142" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A142" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="B140" s="1" t="s">
+      <c r="B142" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="C140" s="1" t="s">
+      <c r="C142" s="1" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A141" s="1" t="s">
+    <row r="143" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A143" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="B141" s="1" t="s">
+      <c r="B143" s="1" t="s">
         <v>346</v>
       </c>
-      <c r="C141" s="1" t="s">
+      <c r="C143" s="1" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A143" s="1" t="s">
+    <row r="145" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A145" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="B143" s="1" t="s">
+      <c r="B145" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="C143" s="1" t="s">
+      <c r="C145" s="1" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A144" s="1" t="s">
+    <row r="146" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A146" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="B144" s="1" t="s">
+      <c r="B146" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="C144" s="1" t="s">
+      <c r="C146" s="1" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A146" s="1" t="s">
+    <row r="148" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A148" s="1" t="s">
         <v>363</v>
       </c>
-      <c r="B146" s="1" t="s">
+      <c r="B148" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="C146" s="1" t="s">
+      <c r="C148" s="1" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A147" s="1" t="s">
+    <row r="149" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A149" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="B147" s="1" t="s">
+      <c r="B149" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="C147" s="1" t="s">
+      <c r="C149" s="1" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A148" s="1" t="s">
+    <row r="150" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A150" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="B148" t="s">
+      <c r="B150" t="s">
         <v>355</v>
       </c>
-      <c r="C148" s="1" t="s">
+      <c r="C150" s="1" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A150" s="1" t="s">
+    <row r="152" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A152" s="1" t="s">
         <v>370</v>
       </c>
-      <c r="B150" t="s">
+      <c r="B152" t="s">
         <v>374</v>
       </c>
-      <c r="C150" s="1" t="s">
+      <c r="C152" s="1" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A151" s="1" t="s">
+    <row r="153" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A153" s="1" t="s">
         <v>371</v>
       </c>
-      <c r="B151" t="s">
+      <c r="B153" t="s">
         <v>373</v>
       </c>
-      <c r="C151" s="1" t="s">
+      <c r="C153" s="1" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A152" s="1" t="s">
+    <row r="154" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A154" s="1" t="s">
         <v>376</v>
       </c>
-      <c r="B152" t="s">
+      <c r="B154" t="s">
         <v>377</v>
       </c>
-      <c r="C152" s="1" t="s">
+      <c r="C154" s="1" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A153" s="1" t="s">
+    <row r="155" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A155" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="B153" t="s">
+      <c r="B155" t="s">
         <v>381</v>
       </c>
-      <c r="C153" s="1" t="s">
+      <c r="C155" s="1" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A154" s="1" t="s">
+    <row r="156" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A156" s="1" t="s">
         <v>379</v>
       </c>
-      <c r="B154" t="s">
+      <c r="B156" t="s">
         <v>380</v>
       </c>
-      <c r="C154" s="1" t="s">
+      <c r="C156" s="1" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A156" s="1" t="s">
+    <row r="158" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A158" s="1" t="s">
         <v>384</v>
       </c>
-      <c r="B156" s="1" t="s">
+      <c r="B158" s="1" t="s">
         <v>385</v>
       </c>
-      <c r="C156" s="1" t="s">
+      <c r="C158" s="1" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A158" s="1" t="s">
+    <row r="160" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A160" s="1" t="s">
         <v>410</v>
       </c>
-      <c r="B158" t="s">
+      <c r="B160" t="s">
         <v>387</v>
       </c>
-      <c r="C158" t="s">
+      <c r="C160" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A159" t="s">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
         <v>389</v>
       </c>
-      <c r="B159" t="s">
+      <c r="B161" t="s">
         <v>391</v>
       </c>
-      <c r="C159" t="s">
+      <c r="C161" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A160" t="s">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A162" t="s">
         <v>390</v>
       </c>
-      <c r="B160" t="s">
+      <c r="B162" t="s">
         <v>392</v>
       </c>
-      <c r="C160" t="s">
+      <c r="C162" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A161" t="s">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A163" t="s">
         <v>395</v>
       </c>
-      <c r="B161" t="s">
+      <c r="B163" t="s">
         <v>396</v>
       </c>
-      <c r="C161" t="s">
+      <c r="C163" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A162" t="s">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A164" t="s">
         <v>398</v>
       </c>
-      <c r="B162" t="s">
+      <c r="B164" t="s">
         <v>400</v>
       </c>
-      <c r="C162" t="s">
+      <c r="C164" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A163" t="s">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A165" t="s">
         <v>403</v>
       </c>
-      <c r="B163" t="s">
+      <c r="B165" t="s">
         <v>401</v>
       </c>
-      <c r="C163" t="s">
+      <c r="C165" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A164" t="s">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A166" t="s">
         <v>406</v>
       </c>
-      <c r="B164" t="s">
+      <c r="B166" t="s">
         <v>404</v>
       </c>
-      <c r="C164" t="s">
+      <c r="C166" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A165" t="s">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A167" t="s">
         <v>407</v>
       </c>
-      <c r="B165" t="s">
+      <c r="B167" t="s">
         <v>408</v>
       </c>
-      <c r="C165" t="s">
+      <c r="C167" t="s">
         <v>409</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A168" t="s">
+        <v>415</v>
+      </c>
+      <c r="B168" t="s">
+        <v>415</v>
+      </c>
+      <c r="C168" t="s">
+        <v>416</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
improved new format remove unused codes changed return codes removed Japanese comments
</commit_message>
<xml_diff>
--- a/Dev/release/resources/Languages.xlsx
+++ b/Dev/release/resources/Languages.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10917"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D943401B-DEC4-3846-979B-F81D7859C83C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="41480" windowHeight="20360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="465" windowWidth="41475" windowHeight="20355"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="424">
   <si>
     <t>AboutEffekseer</t>
   </si>
@@ -1550,22 +1549,50 @@
   <si>
     <t>キャンセル</t>
   </si>
+  <si>
+    <t>EffekseerParticleFilter</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>efkptl</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ProjectFilterNew</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>efkproj,efkptl</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Error_NotFound</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>{0} is not found.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>{0} が見つかりません。</t>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -1601,7 +1628,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -1617,7 +1644,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1692,23 +1719,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1744,23 +1754,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1936,21 +1929,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C168"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
-      <selection activeCell="A168" sqref="A168:C168"/>
+    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
+      <selection activeCell="A138" sqref="A138"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="34.33203125" customWidth="1"/>
-    <col min="2" max="2" width="80.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.375" customWidth="1"/>
+    <col min="2" max="2" width="80.125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="69" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>300</v>
       </c>
@@ -1961,7 +1954,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1972,7 +1965,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1983,7 +1976,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1994,7 +1987,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -2005,7 +1998,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -2016,7 +2009,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -2027,7 +2020,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -2038,7 +2031,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
@@ -2049,7 +2042,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
@@ -2060,7 +2053,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
@@ -2071,7 +2064,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
@@ -2082,7 +2075,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>20</v>
       </c>
@@ -2093,7 +2086,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>21</v>
       </c>
@@ -2104,7 +2097,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>23</v>
       </c>
@@ -2115,7 +2108,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
         <v>24</v>
       </c>
@@ -2126,7 +2119,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
         <v>25</v>
       </c>
@@ -2137,7 +2130,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
         <v>26</v>
       </c>
@@ -2148,7 +2141,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
         <v>27</v>
       </c>
@@ -2159,7 +2152,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
         <v>29</v>
       </c>
@@ -2170,7 +2163,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
         <v>30</v>
       </c>
@@ -2181,7 +2174,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
         <v>32</v>
       </c>
@@ -2192,7 +2185,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
         <v>34</v>
       </c>
@@ -2203,7 +2196,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
         <v>36</v>
       </c>
@@ -2214,7 +2207,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
         <v>38</v>
       </c>
@@ -2225,7 +2218,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
         <v>40</v>
       </c>
@@ -2236,7 +2229,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
         <v>42</v>
       </c>
@@ -2247,7 +2240,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
         <v>43</v>
       </c>
@@ -2258,7 +2251,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
         <v>45</v>
       </c>
@@ -2269,7 +2262,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
         <v>46</v>
       </c>
@@ -2280,7 +2273,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" ht="27" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
         <v>47</v>
       </c>
@@ -2291,7 +2284,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
         <v>49</v>
       </c>
@@ -2302,7 +2295,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
         <v>50</v>
       </c>
@@ -2313,7 +2306,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
         <v>367</v>
       </c>
@@ -2324,7 +2317,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
         <v>52</v>
       </c>
@@ -2335,7 +2328,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
         <v>53</v>
       </c>
@@ -2346,262 +2339,262 @@
         <v>219</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>340</v>
+        <v>56</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A40" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A41" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A42" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A43" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A44" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A45" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A46" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A47" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A49" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A50" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A51" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A52" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A53" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A54" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A55" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A56" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A57" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A58" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A59" s="1" t="s">
-        <v>95</v>
+        <v>414</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>96</v>
+        <v>412</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A60" s="1" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>412</v>
@@ -2610,1095 +2603,1133 @@
         <v>413</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A61" s="1" t="s">
-        <v>411</v>
+        <v>97</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>412</v>
+        <v>97</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A62" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A63" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A64" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A65" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A66" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A67" s="1" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A68" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A69" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A70" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A71" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A72" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A73" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A74" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A75" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A76" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A77" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A78" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A79" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A80" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A81" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A82" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A83" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A84" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A85" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A86" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A87" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A88" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A89" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A90" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A91" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A92" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A93" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A94" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A95" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A96" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A97" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A98" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A99" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A100" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A101" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A102" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A103" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A104" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A105" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A106" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A107" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A108" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A109" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A110" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A111" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A112" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A113" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A114" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A115" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A116" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A117" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A118" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A119" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A120" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A121" s="1"/>
+      <c r="B121" s="1"/>
+      <c r="C121" s="1"/>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A122" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A123" s="1"/>
+      <c r="B123" s="1"/>
+      <c r="C123" s="1"/>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A124" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" ht="27" x14ac:dyDescent="0.15">
+      <c r="A125" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A126" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" ht="27" x14ac:dyDescent="0.15">
+      <c r="A127" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A128" s="1"/>
+      <c r="B128" s="2"/>
+      <c r="C128" s="1"/>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A129" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="C129" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A130" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="C130" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A131" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A132" s="1"/>
+      <c r="B132" s="1"/>
+      <c r="C132" s="1"/>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A133" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A134" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A135" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A136" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A137" s="1"/>
+      <c r="B137" s="1"/>
+      <c r="C137" s="1"/>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A138" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A139" s="1"/>
+      <c r="B139" s="1"/>
+      <c r="C139" s="1"/>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A140" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A141" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A142" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A143" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B68" s="1" t="s">
+      <c r="B143" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="C68" s="1" t="s">
+      <c r="C143" s="1" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A69" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A70" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A71" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A72" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A73" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A74" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A75" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A76" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A77" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A78" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A79" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A80" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B80" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A81" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A82" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="C82" s="1" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A83" s="1" t="s">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A144" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B83" s="1" t="s">
+      <c r="B144" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="C83" s="1" t="s">
+      <c r="C144" s="1" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="84" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A84" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="B84" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C84" s="1" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A85" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C85" s="1" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A86" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A87" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="B87" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="C87" s="1" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A88" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="B88" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A89" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="B89" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C89" s="1" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A90" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="B90" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C90" s="1" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A91" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B91" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="C91" s="1" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A92" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="B92" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A93" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="B93" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="C93" s="1" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A94" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="B94" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="C94" s="1" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A95" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="B95" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="C95" s="1" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A96" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="B96" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A97" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="B97" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C97" s="1" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A98" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="B98" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="C98" s="1" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A99" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="B99" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="C99" s="1" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A100" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="B100" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="C100" s="1" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A101" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="B101" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C101" s="1" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A102" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="B102" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="C102" s="1" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A103" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="B103" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="C103" s="1" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A104" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="B104" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="C104" s="1" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A105" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="B105" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="C105" s="1" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A106" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="B106" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="C106" s="1" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A107" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="B107" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="C107" s="1" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A108" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="B108" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="C108" s="1" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A109" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="B109" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="C109" s="1" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A110" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="B110" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="C110" s="1" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A111" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="B111" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="C111" s="1" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A112" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="B112" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="C112" s="1" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A113" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="B113" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="C113" s="1" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A114" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="B114" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="C114" s="1" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A115" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="B115" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="C115" s="1" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A116" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="B116" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="C116" s="1" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A117" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="B117" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="C117" s="1" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A118" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="B118" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="C118" s="1" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A119" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="B119" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="C119" s="1" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A120" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="B120" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="C120" s="1" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A121" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="B121" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="C121" s="1" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A122" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="B122" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="C122" s="1" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A123" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="B123" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="C123" s="1" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A124" s="1"/>
-      <c r="B124" s="1"/>
-      <c r="C124" s="1"/>
-    </row>
-    <row r="125" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A125" s="1" t="s">
-        <v>366</v>
-      </c>
-      <c r="B125" s="1" t="s">
-        <v>364</v>
-      </c>
-      <c r="C125" s="1" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A126" s="1"/>
-      <c r="B126" s="1"/>
-      <c r="C126" s="1"/>
-    </row>
-    <row r="127" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A127" s="1" t="s">
-        <v>322</v>
-      </c>
-      <c r="B127" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="C127" s="1" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A128" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="B128" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="C128" s="1" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A129" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="B129" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="C129" s="1" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A130" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="B130" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="C130" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A131" s="1"/>
-      <c r="B131" s="2"/>
-      <c r="C131" s="1"/>
-    </row>
-    <row r="132" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A132" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="B132" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="C132" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A133" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="B133" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="C133" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A134" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="B134" s="1" t="s">
-        <v>334</v>
-      </c>
-      <c r="C134" s="1" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A135" s="1"/>
-      <c r="B135" s="1"/>
-      <c r="C135" s="1"/>
-    </row>
-    <row r="136" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A136" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="B136" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C136" s="1" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A137" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="B137" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C137" s="1" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A138" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="B138" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C138" s="1" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A139" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="B139" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="C139" s="1" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A140" s="1"/>
-      <c r="B140" s="1"/>
-      <c r="C140" s="1"/>
-    </row>
-    <row r="142" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A142" s="1" t="s">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A145" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="C145" s="1" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A147" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="B142" s="1" t="s">
+      <c r="B147" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="C142" s="1" t="s">
+      <c r="C147" s="1" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="143" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A143" s="1" t="s">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A148" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="B143" s="1" t="s">
+      <c r="B148" s="1" t="s">
         <v>346</v>
       </c>
-      <c r="C143" s="1" t="s">
+      <c r="C148" s="1" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="145" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A145" s="1" t="s">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A150" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="B145" s="1" t="s">
+      <c r="B150" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="C145" s="1" t="s">
+      <c r="C150" s="1" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="146" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A146" s="1" t="s">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A151" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="B146" s="1" t="s">
+      <c r="B151" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="C146" s="1" t="s">
+      <c r="C151" s="1" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="148" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A148" s="1" t="s">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A153" s="1" t="s">
         <v>363</v>
       </c>
-      <c r="B148" s="1" t="s">
+      <c r="B153" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="C148" s="1" t="s">
+      <c r="C153" s="1" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="149" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A149" s="1" t="s">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A154" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="B149" s="1" t="s">
+      <c r="B154" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="C149" s="1" t="s">
+      <c r="C154" s="1" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="150" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A150" s="1" t="s">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A155" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="B150" t="s">
+      <c r="B155" t="s">
         <v>355</v>
       </c>
-      <c r="C150" s="1" t="s">
+      <c r="C155" s="1" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="152" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A152" s="1" t="s">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A157" s="1" t="s">
         <v>370</v>
       </c>
-      <c r="B152" t="s">
+      <c r="B157" t="s">
         <v>374</v>
       </c>
-      <c r="C152" s="1" t="s">
+      <c r="C157" s="1" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="153" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A153" s="1" t="s">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A158" s="1" t="s">
         <v>371</v>
       </c>
-      <c r="B153" t="s">
+      <c r="B158" t="s">
         <v>373</v>
       </c>
-      <c r="C153" s="1" t="s">
+      <c r="C158" s="1" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="154" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A154" s="1" t="s">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A159" s="1" t="s">
         <v>376</v>
       </c>
-      <c r="B154" t="s">
+      <c r="B159" t="s">
         <v>377</v>
       </c>
-      <c r="C154" s="1" t="s">
+      <c r="C159" s="1" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="155" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A155" s="1" t="s">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A160" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="B155" t="s">
+      <c r="B160" t="s">
         <v>381</v>
       </c>
-      <c r="C155" s="1" t="s">
+      <c r="C160" s="1" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="156" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A156" s="1" t="s">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A161" s="1" t="s">
         <v>379</v>
       </c>
-      <c r="B156" t="s">
+      <c r="B161" t="s">
         <v>380</v>
       </c>
-      <c r="C156" s="1" t="s">
+      <c r="C161" s="1" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="158" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A158" s="1" t="s">
-        <v>384</v>
-      </c>
-      <c r="B158" s="1" t="s">
-        <v>385</v>
-      </c>
-      <c r="C158" s="1" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="160" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A160" s="1" t="s">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A164" s="1" t="s">
         <v>410</v>
       </c>
-      <c r="B160" t="s">
+      <c r="B164" t="s">
         <v>387</v>
       </c>
-      <c r="C160" t="s">
+      <c r="C164" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A161" t="s">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A165" t="s">
         <v>389</v>
       </c>
-      <c r="B161" t="s">
+      <c r="B165" t="s">
         <v>391</v>
       </c>
-      <c r="C161" t="s">
+      <c r="C165" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A162" t="s">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A166" t="s">
         <v>390</v>
       </c>
-      <c r="B162" t="s">
+      <c r="B166" t="s">
         <v>392</v>
       </c>
-      <c r="C162" t="s">
+      <c r="C166" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A163" t="s">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A167" t="s">
         <v>395</v>
       </c>
-      <c r="B163" t="s">
+      <c r="B167" t="s">
         <v>396</v>
       </c>
-      <c r="C163" t="s">
+      <c r="C167" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A164" t="s">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A168" t="s">
         <v>398</v>
       </c>
-      <c r="B164" t="s">
+      <c r="B168" t="s">
         <v>400</v>
       </c>
-      <c r="C164" t="s">
+      <c r="C168" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A165" t="s">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A169" t="s">
         <v>403</v>
       </c>
-      <c r="B165" t="s">
+      <c r="B169" t="s">
         <v>401</v>
       </c>
-      <c r="C165" t="s">
+      <c r="C169" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A166" t="s">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A170" t="s">
         <v>406</v>
       </c>
-      <c r="B166" t="s">
+      <c r="B170" t="s">
         <v>404</v>
       </c>
-      <c r="C166" t="s">
+      <c r="C170" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A167" t="s">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A171" t="s">
         <v>407</v>
       </c>
-      <c r="B167" t="s">
+      <c r="B171" t="s">
         <v>408</v>
       </c>
-      <c r="C167" t="s">
+      <c r="C171" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A168" t="s">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A172" t="s">
         <v>415</v>
       </c>
-      <c r="B168" t="s">
+      <c r="B172" t="s">
         <v>415</v>
       </c>
-      <c r="C168" t="s">
+      <c r="C172" t="s">
         <v>416</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added reserved parameters fixed new formats
</commit_message>
<xml_diff>
--- a/Dev/release/resources/Languages.xlsx
+++ b/Dev/release/resources/Languages.xlsx
@@ -1554,18 +1554,10 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>efkptl</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>ProjectFilterNew</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>efkproj,efkptl</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Error_NotFound</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -1576,6 +1568,12 @@
   <si>
     <t>{0} が見つかりません。</t>
     <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>efkefc</t>
+  </si>
+  <si>
+    <t>efkproj,efkefc</t>
   </si>
 </sst>
 </file>
@@ -1933,7 +1931,7 @@
   <dimension ref="A1:C172"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
-      <selection activeCell="A138" sqref="A138"/>
+      <selection activeCell="C143" sqref="C143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3422,13 +3420,13 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A138" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="C138" s="1" t="s">
         <v>421</v>
-      </c>
-      <c r="B138" s="1" t="s">
-        <v>422</v>
-      </c>
-      <c r="C138" s="1" t="s">
-        <v>423</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.15">
@@ -3441,10 +3439,10 @@
         <v>417</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>418</v>
+        <v>422</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>418</v>
+        <v>422</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.15">
@@ -3493,13 +3491,13 @@
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A145" s="1" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>420</v>
+        <v>423</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>420</v>
+        <v>423</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
rename post effect -> environement
</commit_message>
<xml_diff>
--- a/Dev/release/resources/Languages.xlsx
+++ b/Dev/release/resources/Languages.xlsx
@@ -1148,18 +1148,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>PostEffect</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>PostEffect</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ポストエフェクト</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Clipping</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -1574,6 +1562,21 @@
   </si>
   <si>
     <t>efkproj,efkefc</t>
+  </si>
+  <si>
+    <t>Environment_Name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Environment</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>環境</t>
+    <rPh sb="0" eb="2">
+      <t>カンキョウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
@@ -1928,10 +1931,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C172"/>
+  <dimension ref="A1:C174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
-      <selection activeCell="C143" sqref="C143"/>
+    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
+      <selection activeCell="C175" sqref="C175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2026,7 +2029,7 @@
         <v>12</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
@@ -2306,13 +2309,13 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.15">
@@ -2581,24 +2584,24 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A59" s="1" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A60" s="1" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.15">
@@ -3268,13 +3271,13 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A122" s="1" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.15">
@@ -3420,13 +3423,13 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A138" s="1" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.15">
@@ -3436,24 +3439,24 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A140" s="1" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A141" s="1" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.15">
@@ -3491,244 +3494,244 @@
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A145" s="1" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A147" s="1" t="s">
-        <v>342</v>
-      </c>
-      <c r="B147" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="C147" s="1" t="s">
-        <v>344</v>
+        <v>420</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A148" s="1" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A150" s="1" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="B150" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="C150" s="1" t="s">
         <v>349</v>
-      </c>
-      <c r="C150" s="1" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A151" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="C151" s="1" t="s">
         <v>350</v>
-      </c>
-      <c r="B151" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="C151" s="1" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A153" s="1" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A154" s="1" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A155" s="1" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="B155" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A157" s="1" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="B157" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A158" s="1" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="B158" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A159" s="1" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="B159" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A160" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="B160" t="s">
         <v>378</v>
       </c>
-      <c r="B160" t="s">
-        <v>381</v>
-      </c>
       <c r="C160" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A161" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="B161" t="s">
+        <v>377</v>
+      </c>
+      <c r="C161" s="1" t="s">
         <v>380</v>
-      </c>
-      <c r="C161" s="1" t="s">
-        <v>383</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A164" s="1" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="B164" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="C164" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A165" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="B165" t="s">
+        <v>388</v>
+      </c>
+      <c r="C165" t="s">
         <v>391</v>
-      </c>
-      <c r="C165" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A166" t="s">
+        <v>387</v>
+      </c>
+      <c r="B166" t="s">
+        <v>389</v>
+      </c>
+      <c r="C166" t="s">
         <v>390</v>
-      </c>
-      <c r="B166" t="s">
-        <v>392</v>
-      </c>
-      <c r="C166" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A167" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="B167" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="C167" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A168" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="B168" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="C168" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A169" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="B169" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="C169" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A170" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="B170" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="C170" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A171" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="B171" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C171" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A172" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="B172" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="C172" t="s">
-        <v>416</v>
+        <v>413</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A174" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="B174" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="C174" s="1" t="s">
+        <v>423</v>
       </c>
     </row>
   </sheetData>

</xml_diff>